<commit_message>
auto: publish 18-10-2025  0:45:47,52
</commit_message>
<xml_diff>
--- a/Template_Proyectos_Dashboard.xlsx
+++ b/Template_Proyectos_Dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\dashboard-proyectos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02E92DB-F775-4D26-B442-FBC041D45944}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{415BDA2D-7AAD-4DC7-9004-1502178C757B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4680" yWindow="-16320" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Proyectos" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="193">
   <si>
     <t>Tipo</t>
   </si>
@@ -117,9 +117,6 @@
     <t>Check Persons/Komatsu</t>
   </si>
   <si>
-    <t>Legacy 2</t>
-  </si>
-  <si>
     <t>Propuesta enviada ($5.700.000)</t>
   </si>
   <si>
@@ -486,9 +483,6 @@
     <t>Armar presentación visual</t>
   </si>
   <si>
-    <t>Legacy Operaciones (2 roles)</t>
-  </si>
-  <si>
     <t>Armar Gantt y validar</t>
   </si>
   <si>
@@ -622,6 +616,9 @@
   </si>
   <si>
     <t>Legacy x2 ( Luis + Jaime)</t>
+  </si>
+  <si>
+    <t>Armar propuesta Técnica</t>
   </si>
 </sst>
 </file>
@@ -1119,11 +1116,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H122"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G130" sqref="G130"/>
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C129" sqref="C129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1164,7 +1162,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1190,7 +1188,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1216,7 +1214,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -1242,7 +1240,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -1268,7 +1266,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -1276,10 +1274,10 @@
         <v>24</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="E6" s="3">
         <v>45915</v>
@@ -1294,18 +1292,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E7" s="3">
         <v>45915</v>
@@ -1320,18 +1318,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" s="3">
         <v>45915</v>
@@ -1346,15 +1344,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>23</v>
@@ -1372,18 +1370,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="E10" s="3">
         <v>45915</v>
@@ -1398,18 +1396,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>37</v>
       </c>
       <c r="E11" s="3">
         <v>45915</v>
@@ -1424,18 +1422,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="E12" s="3">
         <v>45923</v>
@@ -1450,18 +1448,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E13" s="3">
         <v>45923</v>
@@ -1476,18 +1474,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="E14" s="3">
         <v>45929</v>
@@ -1502,7 +1500,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
@@ -1510,10 +1508,10 @@
         <v>21</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="E15" s="3">
         <v>45931</v>
@@ -1528,18 +1526,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="D16" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E16" s="3">
         <v>45932</v>
@@ -1554,76 +1552,76 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="D17" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E17" s="3">
         <v>45940</v>
       </c>
       <c r="F17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="H17" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="E18" s="3">
         <v>45933</v>
       </c>
       <c r="F18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="G18" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="E19" s="3">
         <v>45933</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G19" s="9" t="s">
         <v>13</v>
@@ -1632,111 +1630,111 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="D20" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E20" s="3">
         <v>45950</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G20" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H20" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="E21" s="3">
         <v>45950</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H21" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E22" s="3">
         <v>45950</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H22" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E23" s="3">
         <v>45950</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H23" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>2</v>
       </c>
@@ -1744,10 +1742,10 @@
         <v>21</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E24" s="3">
         <v>45936</v>
@@ -1762,18 +1760,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="D25" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E25" s="3">
         <v>45936</v>
@@ -1788,18 +1786,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="D26" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E26" s="3">
         <v>45936</v>
@@ -1814,50 +1812,50 @@
         <v>14</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E27" s="3">
         <v>45940</v>
       </c>
       <c r="F27" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G27" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H27" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="E28" s="3">
         <v>45940</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G28" s="9" t="s">
         <v>13</v>
@@ -1866,70 +1864,70 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E29" s="3">
         <v>45950</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H29" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E30" s="3">
         <v>45950</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G30" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="H30" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>187</v>
       </c>
       <c r="E31" s="3">
         <v>45940</v>
@@ -1944,24 +1942,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="D32" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E32" s="3">
         <v>45963</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G32" s="3" t="s">
         <v>13</v>
@@ -1975,13 +1973,13 @@
         <v>8</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E33" s="3">
         <v>45937</v>
@@ -1990,24 +1988,24 @@
         <v>12</v>
       </c>
       <c r="G33" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H33" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="D34" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E34" s="3">
         <v>45943</v>
@@ -2016,24 +2014,24 @@
         <v>12</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H34" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="D35" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E35" s="3">
         <v>45943</v>
@@ -2048,18 +2046,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="D36" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E36" s="3">
         <v>45936</v>
@@ -2068,82 +2066,82 @@
         <v>12</v>
       </c>
       <c r="G36" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="H36" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="H36" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="E37" s="3">
         <v>45947</v>
       </c>
       <c r="F37" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G37" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H37" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B38" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="D38" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E38" s="3">
         <v>45947</v>
       </c>
       <c r="F38" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G38" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H38" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="D39" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E39" s="3">
         <v>45947</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G39" s="9" t="s">
         <v>13</v>
@@ -2152,76 +2150,76 @@
         <v>14</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E40" s="3">
         <v>45950</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G40" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H40" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E41" s="3">
         <v>45950</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H41" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C42" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="D42" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E42" s="3">
         <v>45963</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G42" s="3" t="s">
         <v>13</v>
@@ -2230,18 +2228,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="D43" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E43" s="3">
         <v>45943</v>
@@ -2256,50 +2254,50 @@
         <v>14</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="D44" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E44" s="3">
         <v>45950</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G44" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H44" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E45" s="3">
         <v>45954</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G45" s="9" t="s">
         <v>13</v>
@@ -2308,24 +2306,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E46" s="3">
         <v>45954</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G46" s="9" t="s">
         <v>13</v>
@@ -2334,18 +2332,18 @@
         <v>14</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="D47" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E47" s="3">
         <v>45943</v>
@@ -2354,30 +2352,30 @@
         <v>12</v>
       </c>
       <c r="G47" s="9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H47" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="D48" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E48" s="3">
         <v>45966</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G48" s="9" t="s">
         <v>13</v>
@@ -2386,50 +2384,50 @@
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B49" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C49" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="D49" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E49" s="3">
         <v>45963</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H49" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B50" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C50" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="D50" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E50" s="3">
         <v>45961</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G50" s="3" t="s">
         <v>13</v>
@@ -2438,24 +2436,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="D51" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E51" s="3">
         <v>45961</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>13</v>
@@ -2464,24 +2462,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B52" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="D52" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E52" s="3">
         <v>45961</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>13</v>
@@ -2490,50 +2488,50 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B53" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="D53" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E53" s="3">
         <v>45971</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H53" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B54" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="D54" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E54" s="3">
         <v>45971</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G54" s="9" t="s">
         <v>13</v>
@@ -2542,24 +2540,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E55" s="3">
         <v>45968</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G55" s="9" t="s">
         <v>13</v>
@@ -2568,76 +2566,76 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="D56" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E56" s="3">
         <v>45971</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H56" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C57" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="D57" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E57" s="3">
         <v>45965</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H57" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B58" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="D58" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E58" s="3">
         <v>45978</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G58" s="9" t="s">
         <v>13</v>
@@ -2646,50 +2644,50 @@
         <v>14</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B59" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C59" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="D59" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E59" s="3">
         <v>45966</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G59" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H59" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E60" s="3">
         <v>45975</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G60" s="9" t="s">
         <v>13</v>
@@ -2698,24 +2696,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E61" s="3">
         <v>45982</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G61" s="9" t="s">
         <v>13</v>
@@ -2724,24 +2722,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E62" s="3">
         <v>45989</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G62" s="9" t="s">
         <v>13</v>
@@ -2750,24 +2748,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B63" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="D63" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>103</v>
       </c>
       <c r="E63" s="3">
         <v>45943</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G63" s="9" t="s">
         <v>13</v>
@@ -2776,50 +2774,50 @@
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B64" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C64" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C64" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="D64" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E64" s="3">
         <v>45968</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H64" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B65" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C65" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C65" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="D65" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E65" s="3">
         <v>45978</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G65" s="3" t="s">
         <v>13</v>
@@ -2828,241 +2826,241 @@
         <v>14</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C66" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="D66" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E66" s="3">
         <v>45978</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H66" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E67" s="3">
         <v>45985</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H67" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E68" s="3">
         <v>45985</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H68" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E69" s="3">
         <v>45985</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H69" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E70" s="3">
         <v>45985</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H70" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B71" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C71" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C71" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="D71" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E71" s="3">
         <v>45957</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G71" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H71" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E72" s="3">
         <v>45985</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H72" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E73" s="3">
         <v>45985</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H73" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A74" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E74" s="3">
         <v>45985</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="H74" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A75" s="2" t="s">
         <v>8</v>
       </c>
@@ -3070,16 +3068,16 @@
         <v>24</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>25</v>
+        <v>191</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E75" s="3">
         <v>45944</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>123</v>
+        <v>12</v>
       </c>
       <c r="G75" s="9" t="s">
         <v>13</v>
@@ -3093,45 +3091,45 @@
         <v>8</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E76" s="3">
         <v>45947</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G76" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H76" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B77" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C77" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C77" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="D77" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E77" s="3">
         <v>45947</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G77" s="9" t="s">
         <v>13</v>
@@ -3140,7 +3138,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="2" t="s">
         <v>8</v>
       </c>
@@ -3151,13 +3149,13 @@
         <v>19</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E78" s="3">
         <v>45950</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G78" s="9" t="s">
         <v>13</v>
@@ -3166,180 +3164,180 @@
         <v>14</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B79" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C79" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="D79" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="D79" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="E79" s="3">
         <v>45944</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G79" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H79" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B80" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C80" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C80" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="D80" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E80" s="3">
         <v>45947</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G80" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H80" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B81" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C81" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C81" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="D81" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E81" s="3">
         <v>45950</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G81" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H81" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B82" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C82" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C82" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="D82" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E82" s="3">
         <v>45957</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G82" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H82" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B83" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C83" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C83" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="D83" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E83" s="3">
         <v>45960</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G83" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H83" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B84" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C84" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C84" s="2" t="s">
-        <v>133</v>
-      </c>
       <c r="D84" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E84" s="3">
         <v>45975</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G84" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H84" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C85" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D85" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>141</v>
       </c>
       <c r="E85" s="13">
         <v>45947</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G85" s="2" t="s">
         <v>13</v>
@@ -3348,44 +3346,44 @@
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B86" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C86" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C86" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="D86" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E86" s="3">
         <v>45950</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H86" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B87" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C87" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C87" s="2" t="s">
+      <c r="D87" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="E87" s="13">
         <v>45946</v>
@@ -3394,30 +3392,30 @@
         <v>12</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H87" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>148</v>
+        <v>191</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E88" s="13">
         <v>45945</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
       <c r="G88" s="3" t="s">
         <v>13</v>
@@ -3426,856 +3424,856 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E89" s="13">
         <v>45945</v>
       </c>
       <c r="F89" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H89" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G89" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H89" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A90" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C90" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E90" s="13">
         <v>45950</v>
       </c>
       <c r="F90" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H90" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B91" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G90" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H90" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A91" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C91" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E91" s="13">
         <v>45954</v>
       </c>
       <c r="F91" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H91" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B92" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G91" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H91" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A92" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B92" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C92" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E92" s="13">
         <v>45957</v>
       </c>
       <c r="F92" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H92" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B93" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G92" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H92" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A93" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C93" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E93" s="13">
         <v>45957</v>
       </c>
       <c r="F93" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G93" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H93" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G93" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H93" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A94" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B94" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C94" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E94" s="13">
         <v>45957</v>
       </c>
       <c r="F94" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H94" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B95" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G94" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H94" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A95" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C95" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E95" s="13">
         <v>45964</v>
       </c>
       <c r="F95" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H95" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B96" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G95" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H95" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A96" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C96" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E96" s="13">
         <v>45964</v>
       </c>
       <c r="F96" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H96" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G96" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H96" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A97" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B97" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C97" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E97" s="13">
         <v>45971</v>
       </c>
       <c r="F97" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H97" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G97" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H97" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A98" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C98" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E98" s="13">
         <v>45971</v>
       </c>
       <c r="F98" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H98" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B99" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G98" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H98" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A99" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C99" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E99" s="13">
         <v>45971</v>
       </c>
       <c r="F99" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H99" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B100" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G99" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H99" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A100" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C100" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E100" s="13">
         <v>45971</v>
       </c>
       <c r="F100" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H100" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G100" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H100" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A101" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C101" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E101" s="13">
         <v>45978</v>
       </c>
       <c r="F101" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H101" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B102" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G101" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H101" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A102" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C102" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E102" s="13">
         <v>45978</v>
       </c>
       <c r="F102" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H102" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B103" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G102" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H102" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A103" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C103" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E103" s="13">
         <v>45978</v>
       </c>
       <c r="F103" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G103" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H103" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B104" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G103" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H103" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A104" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C104" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D104" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E104" s="13">
         <v>45978</v>
       </c>
       <c r="F104" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H104" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B105" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G104" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H104" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A105" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C105" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E105" s="13">
         <v>45985</v>
       </c>
       <c r="F105" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G105" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H105" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B106" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G105" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H105" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A106" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C106" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E106" s="13">
         <v>45985</v>
       </c>
       <c r="F106" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G106" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H106" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B107" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G106" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H106" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A107" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C107" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D107" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E107" s="13">
         <v>45985</v>
       </c>
       <c r="F107" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G107" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H107" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B108" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G107" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H107" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A108" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C108" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E108" s="13">
         <v>45985</v>
       </c>
       <c r="F108" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H108" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B109" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G108" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H108" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A109" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B109" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C109" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E109" s="13">
         <v>45992</v>
       </c>
       <c r="F109" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G109" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H109" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B110" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G109" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H109" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A110" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B110" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C110" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E110" s="13">
         <v>46027</v>
       </c>
       <c r="F110" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H110" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B111" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G110" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H110" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A111" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C111" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E111" s="13">
         <v>46027</v>
       </c>
       <c r="F111" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G111" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H111" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B112" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G111" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H111" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A112" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C112" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E112" s="13">
         <v>46027</v>
       </c>
       <c r="F112" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G112" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H112" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B113" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G112" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H112" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A113" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C113" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E113" s="13">
         <v>46041</v>
       </c>
       <c r="F113" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G113" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H113" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B114" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G113" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H113" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A114" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C114" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E114" s="13">
         <v>46041</v>
       </c>
       <c r="F114" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G114" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H114" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B115" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G114" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H114" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A115" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C115" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E115" s="13">
         <v>46048</v>
       </c>
       <c r="F115" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G115" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H115" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B116" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G115" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H115" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A116" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C116" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E116" s="13">
         <v>46048</v>
       </c>
       <c r="F116" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H116" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B117" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G116" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H116" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A117" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C117" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E117" s="13">
         <v>46048</v>
       </c>
       <c r="F117" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G117" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H117" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B118" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G117" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H117" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A118" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C118" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E118" s="13">
         <v>46055</v>
       </c>
       <c r="F118" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H118" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B119" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G118" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H118" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A119" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C119" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E119" s="13">
         <v>46055</v>
       </c>
       <c r="F119" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G119" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H119" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B120" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G119" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H119" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A120" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C120" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E120" s="13">
         <v>46062</v>
       </c>
       <c r="F120" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H120" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A121" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B121" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="G120" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H120" s="12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A121" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B121" s="2" t="s">
-        <v>65</v>
-      </c>
       <c r="C121" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E121" s="13">
         <v>46174</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G121" s="3" t="s">
         <v>13</v>
@@ -4284,34 +4282,65 @@
         <v>14</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B122" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C122" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="C122" s="2" t="s">
-        <v>146</v>
-      </c>
       <c r="D122" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E122" s="13">
         <v>45950</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H122" s="12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A123" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D123" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="E123" s="3">
+        <v>45951</v>
+      </c>
+      <c r="F123" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="G123" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H123" s="12" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H122" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Licitación modelo gestión instructores"/>
+      </filters>
+    </filterColumn>
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:H74">
       <sortCondition ref="E1:E122"/>
     </sortState>
@@ -4337,6 +4366,7 @@
     <hyperlink ref="H56" r:id="rId15" display="mailto:msuarez@schilling.cl" xr:uid="{AEE2429E-8C99-4585-916D-CE1A1FEC1B4F}"/>
     <hyperlink ref="H57" r:id="rId16" display="mailto:msuarez@schilling.cl" xr:uid="{2F2FB24F-8FD1-4DD9-ACDB-6BF1174D456D}"/>
     <hyperlink ref="H64" r:id="rId17" display="mailto:msuarez@schilling.cl" xr:uid="{D45F3DD8-EA67-4DCC-B92C-B884ED913682}"/>
+    <hyperlink ref="H123" r:id="rId18" display="Loreto.naranjo@gmail.com" xr:uid="{900F514B-C93B-4103-B7A9-A4E7C1DEF677}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -4357,82 +4387,82 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>